<commit_message>
v1.4.6+40: now in spanish and polish
</commit_message>
<xml_diff>
--- a/assets/i18n_data/foods_lang.xlsx
+++ b/assets/i18n_data/foods_lang.xlsx
@@ -2408,7 +2408,7 @@
     <t>Arándano rojo, Arándano rojo, Arándano rojo, Arándano de montaña</t>
   </si>
   <si>
-    <t>lechuga</t>
+    <t>Lechuga</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Litchi_chinensis</t>
@@ -3241,12 +3241,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3270,9 +3270,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3283,11 +3283,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3329,6 +3343,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -3345,22 +3383,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3374,39 +3397,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3421,7 +3414,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3433,13 +3444,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3451,7 +3462,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3463,7 +3534,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3475,133 +3594,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3659,16 +3652,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -3698,16 +3691,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -3715,145 +3708,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -7906,8 +7899,8 @@
   <sheetPr/>
   <dimension ref="B1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
fixed small issues with food data (#82, 81, 76)
</commit_message>
<xml_diff>
--- a/assets/i18n_data/foods_lang.xlsx
+++ b/assets/i18n_data/foods_lang.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="1071">
   <si>
     <t>id</t>
   </si>
@@ -1181,7 +1181,7 @@
     <t>https://en.wikipedia.org/wiki/Kale</t>
   </si>
   <si>
-    <t>Green cabbage, Cabbage, Leaf cabbage, Kale</t>
+    <t>Kale, Green cabbage, Cabbage, Leaf cabbage</t>
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/Allium_fistulosum</t>
@@ -2174,7 +2174,7 @@
     <t>https://es.wikipedia.org/wiki/Ceratonia_siliqua</t>
   </si>
   <si>
-    <t>Carambola, carambola</t>
+    <t>Algarroba</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Daucus_carota</t>
@@ -2201,7 +2201,7 @@
     <t>https://es.wikipedia.org/wiki/Agaricus</t>
   </si>
   <si>
-    <t>Champiñón, Champiñón</t>
+    <t>Champiñón</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Beta_vulgaris_var._cicla</t>
@@ -2237,19 +2237,19 @@
     <t>https://es.wikipedia.org/wiki/Citrus_reticulata</t>
   </si>
   <si>
-    <t>Clementina, Mandarina, Tangor, Mandarina</t>
+    <t>Clementina, Mandarina, Tangor</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Rubus_chamaemorus</t>
   </si>
   <si>
-    <t>Baya nórdica, Baya nórdica, Bakeapple, Knotberry, Knoutberry, Aqpik, Averin, Evron</t>
+    <t>Baya nórdica, Bakeapple, Knotberry, Knoutberry, Aqpik, Averin, Evron</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Cocos_nucifera</t>
   </si>
   <si>
-    <t>Coco, Coco</t>
+    <t>Coco</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Vaccinium_macrocarpon</t>
@@ -2285,7 +2285,7 @@
     <t>https://es.wikipedia.org/wiki/Solanum_melongena</t>
   </si>
   <si>
-    <t>Berenjena, berenjena, berenjena</t>
+    <t>Berenjena</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Sambucus_nigra</t>
@@ -2321,7 +2321,7 @@
     <t>https://es.wikipedia.org/wiki/Citrus_%C3%97_paradisi</t>
   </si>
   <si>
-    <t>Grosella</t>
+    <t>Grosella espinosa europea, uva espina, grosella</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Citrus_maxima</t>
@@ -2360,13 +2360,13 @@
     <t>Guayaba, Psidium Guayaba</t>
   </si>
   <si>
-    <t>Lechuga, Lechuga, Ensalada, Mantequilla, Boston, Lechuga Bibb</t>
+    <t>Lechuga, Ensalada, Mantequilla, Boston, Lechuga Bibb</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Cucumis_melo</t>
   </si>
   <si>
-    <t>Melón verde</t>
+    <t>Melón</t>
   </si>
   <si>
     <t>Ensalada Iceberg, Crisphead, Ensalada, Lechuga</t>
@@ -2375,9 +2375,6 @@
     <t>https://es.wikipedia.org/wiki/Kiwi_(fruto)</t>
   </si>
   <si>
-    <t>Kiwi, kiwi</t>
-  </si>
-  <si>
     <t>https://es.wikipedia.org/wiki/Brassica_oleracea_var._gongylodes</t>
   </si>
   <si>
@@ -2405,7 +2402,7 @@
     <t>https://es.wikipedia.org/wiki/Vaccinium_vitis-idaea</t>
   </si>
   <si>
-    <t>Arándano rojo, Arándano rojo, Arándano rojo, Arándano de montaña</t>
+    <t>Arándano rojo, Arándano de montaña</t>
   </si>
   <si>
     <t>Lechuga</t>
@@ -2447,7 +2444,7 @@
     <t>https://es.wikipedia.org/wiki/Brassica_rapa_subsp._chinensis</t>
   </si>
   <si>
-    <t>Bok choy , col china</t>
+    <t>Bok choy, col china</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Carica_papaya</t>
@@ -2474,7 +2471,7 @@
     <t>https://es.wikipedia.org/wiki/Prunus_persica</t>
   </si>
   <si>
-    <t>Melocotón, durazno</t>
+    <t>Melocotón, durazno, Melocotonero, durazanero</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Pyrus</t>
@@ -2618,13 +2615,13 @@
     <t>https://es.wikipedia.org/wiki/Carambola</t>
   </si>
   <si>
-    <t>Fresa</t>
+    <t>Carambola, fruta de estrella</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Fragaria_%C3%97_ananassa</t>
   </si>
   <si>
-    <t>Camote, Camote</t>
+    <t>Fresa, frutilla, fragaria</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Zea_mays</t>
@@ -2636,7 +2633,7 @@
     <t>https://es.wikipedia.org/wiki/Ipomoea_batatas</t>
   </si>
   <si>
-    <t>Batatas</t>
+    <t>Batata, patata dulce, camote, papa dulce, moniato, boniato</t>
   </si>
   <si>
     <t>https://es.wikipedia.org/wiki/Solanum_lycopersicum</t>
@@ -2645,7 +2642,7 @@
     <t>https://es.wikipedia.org/wiki/Citrullus_lanatus</t>
   </si>
   <si>
-    <t>Sandía, Sandía</t>
+    <t>Sandía, acendría, síndria, patilla, aguamelón, melón de agua</t>
   </si>
   <si>
     <t>Repollo blanco, repollo</t>
@@ -2666,7 +2663,7 @@
     <t>https://es.wikipedia.org/wiki/Calabaza</t>
   </si>
   <si>
-    <t>Calabacín, Calabacín, Tuétano de bebé</t>
+    <t>Calabacín, Tuétano de bebé</t>
   </si>
   <si>
     <t>https://pl.wikipedia.org/wiki/Li%C5%9Bciokwiat_garbnikowy</t>
@@ -3241,10 +3238,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -3269,22 +3266,17 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3295,51 +3287,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3361,7 +3308,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3369,6 +3323,28 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3382,6 +3358,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -3389,17 +3395,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3414,7 +3411,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3432,31 +3459,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3474,7 +3477,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3486,31 +3549,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3522,31 +3573,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3558,43 +3591,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3605,24 +3602,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -3641,6 +3620,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -3652,16 +3655,25 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -3690,160 +3702,145 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5436,8 +5433,8 @@
   <sheetPr/>
   <dimension ref="B1:D101"/>
   <sheetViews>
-    <sheetView topLeftCell="B60" workbookViewId="0">
-      <selection activeCell="L91" sqref="L91"/>
+    <sheetView topLeftCell="B26" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -7899,8 +7896,8 @@
   <sheetPr/>
   <dimension ref="B1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -8455,7 +8452,7 @@
         <v>784</v>
       </c>
       <c r="D50" t="s">
-        <v>785</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="2:4">
@@ -8463,10 +8460,10 @@
         <v>150</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="D51" t="s">
         <v>786</v>
-      </c>
-      <c r="D51" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="52" spans="2:4">
@@ -8474,10 +8471,10 @@
         <v>153</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="D52" t="s">
         <v>788</v>
-      </c>
-      <c r="D52" t="s">
-        <v>789</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -8485,10 +8482,10 @@
         <v>156</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="D53" t="s">
         <v>790</v>
-      </c>
-      <c r="D53" t="s">
-        <v>791</v>
       </c>
     </row>
     <row r="54" spans="2:4">
@@ -8496,10 +8493,10 @@
         <v>159</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="D54" t="s">
         <v>792</v>
-      </c>
-      <c r="D54" t="s">
-        <v>793</v>
       </c>
     </row>
     <row r="55" spans="2:4">
@@ -8507,10 +8504,10 @@
         <v>162</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="D55" t="s">
         <v>794</v>
-      </c>
-      <c r="D55" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="56" spans="2:4">
@@ -8521,7 +8518,7 @@
         <v>705</v>
       </c>
       <c r="D56" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="57" spans="2:4">
@@ -8529,10 +8526,10 @@
         <v>168</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="D57" t="s">
         <v>797</v>
-      </c>
-      <c r="D57" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="58" spans="2:4">
@@ -8540,7 +8537,7 @@
         <v>171</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="D58" t="s">
         <v>173</v>
@@ -8551,10 +8548,10 @@
         <v>174</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="D59" t="s">
         <v>800</v>
-      </c>
-      <c r="D59" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="60" spans="2:4">
@@ -8562,10 +8559,10 @@
         <v>177</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="D60" t="s">
         <v>802</v>
-      </c>
-      <c r="D60" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="61" spans="2:4">
@@ -8573,10 +8570,10 @@
         <v>180</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="D61" t="s">
         <v>804</v>
-      </c>
-      <c r="D61" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="62" spans="2:4">
@@ -8584,10 +8581,10 @@
         <v>183</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="D62" t="s">
         <v>806</v>
-      </c>
-      <c r="D62" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="63" spans="2:4">
@@ -8595,10 +8592,10 @@
         <v>186</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="D63" t="s">
         <v>808</v>
-      </c>
-      <c r="D63" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="64" spans="2:4">
@@ -8606,7 +8603,7 @@
         <v>189</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="D64" t="s">
         <v>423</v>
@@ -8617,10 +8614,10 @@
         <v>192</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="D65" t="s">
         <v>811</v>
-      </c>
-      <c r="D65" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="66" spans="2:4">
@@ -8628,10 +8625,10 @@
         <v>195</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="D66" t="s">
         <v>813</v>
-      </c>
-      <c r="D66" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="67" spans="2:4">
@@ -8639,10 +8636,10 @@
         <v>198</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="D67" t="s">
         <v>815</v>
-      </c>
-      <c r="D67" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="68" spans="2:4">
@@ -8650,10 +8647,10 @@
         <v>201</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="D68" t="s">
         <v>817</v>
-      </c>
-      <c r="D68" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="69" spans="2:4">
@@ -8661,10 +8658,10 @@
         <v>204</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="D69" t="s">
         <v>819</v>
-      </c>
-      <c r="D69" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="70" spans="2:4">
@@ -8672,10 +8669,10 @@
         <v>207</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="D70" t="s">
         <v>821</v>
-      </c>
-      <c r="D70" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="71" spans="2:4">
@@ -8683,10 +8680,10 @@
         <v>210</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="D71" t="s">
         <v>823</v>
-      </c>
-      <c r="D71" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="72" spans="2:4">
@@ -8694,10 +8691,10 @@
         <v>213</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="D72" t="s">
         <v>825</v>
-      </c>
-      <c r="D72" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="73" spans="2:4">
@@ -8705,10 +8702,10 @@
         <v>216</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="D73" t="s">
         <v>827</v>
-      </c>
-      <c r="D73" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="74" spans="2:4">
@@ -8716,10 +8713,10 @@
         <v>219</v>
       </c>
       <c r="C74" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="D74" t="s">
         <v>829</v>
-      </c>
-      <c r="D74" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="75" spans="2:4">
@@ -8727,10 +8724,10 @@
         <v>222</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="D75" t="s">
         <v>831</v>
-      </c>
-      <c r="D75" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="76" spans="2:4">
@@ -8738,10 +8735,10 @@
         <v>225</v>
       </c>
       <c r="C76" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="D76" t="s">
         <v>833</v>
-      </c>
-      <c r="D76" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="77" spans="2:4">
@@ -8749,10 +8746,10 @@
         <v>228</v>
       </c>
       <c r="C77" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="D77" t="s">
         <v>835</v>
-      </c>
-      <c r="D77" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="78" spans="2:4">
@@ -8760,10 +8757,10 @@
         <v>231</v>
       </c>
       <c r="C78" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="D78" t="s">
         <v>837</v>
-      </c>
-      <c r="D78" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="79" spans="2:4">
@@ -8771,10 +8768,10 @@
         <v>234</v>
       </c>
       <c r="C79" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="D79" t="s">
         <v>839</v>
-      </c>
-      <c r="D79" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="80" spans="2:4">
@@ -8782,10 +8779,10 @@
         <v>237</v>
       </c>
       <c r="C80" s="2" t="s">
+        <v>840</v>
+      </c>
+      <c r="D80" t="s">
         <v>841</v>
-      </c>
-      <c r="D80" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="81" spans="2:4">
@@ -8793,10 +8790,10 @@
         <v>240</v>
       </c>
       <c r="C81" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="D81" t="s">
         <v>843</v>
-      </c>
-      <c r="D81" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="82" spans="2:4">
@@ -8804,10 +8801,10 @@
         <v>243</v>
       </c>
       <c r="C82" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="D82" t="s">
         <v>845</v>
-      </c>
-      <c r="D82" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="83" spans="2:4">
@@ -8815,10 +8812,10 @@
         <v>246</v>
       </c>
       <c r="C83" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="D83" t="s">
         <v>847</v>
-      </c>
-      <c r="D83" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="84" spans="2:4">
@@ -8826,10 +8823,10 @@
         <v>249</v>
       </c>
       <c r="C84" s="2" t="s">
+        <v>848</v>
+      </c>
+      <c r="D84" t="s">
         <v>849</v>
-      </c>
-      <c r="D84" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="85" spans="2:4">
@@ -8837,10 +8834,10 @@
         <v>252</v>
       </c>
       <c r="C85" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="D85" t="s">
         <v>851</v>
-      </c>
-      <c r="D85" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="86" spans="2:4">
@@ -8848,10 +8845,10 @@
         <v>255</v>
       </c>
       <c r="C86" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="D86" t="s">
         <v>853</v>
-      </c>
-      <c r="D86" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="87" spans="2:4">
@@ -8859,10 +8856,10 @@
         <v>258</v>
       </c>
       <c r="C87" s="2" t="s">
+        <v>854</v>
+      </c>
+      <c r="D87" t="s">
         <v>855</v>
-      </c>
-      <c r="D87" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="88" spans="2:4">
@@ -8870,10 +8867,10 @@
         <v>261</v>
       </c>
       <c r="C88" s="2" t="s">
+        <v>856</v>
+      </c>
+      <c r="D88" t="s">
         <v>857</v>
-      </c>
-      <c r="D88" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="89" spans="2:4">
@@ -8881,10 +8878,10 @@
         <v>264</v>
       </c>
       <c r="C89" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="D89" t="s">
         <v>859</v>
-      </c>
-      <c r="D89" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="90" spans="2:4">
@@ -8892,10 +8889,10 @@
         <v>267</v>
       </c>
       <c r="C90" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="D90" t="s">
         <v>861</v>
-      </c>
-      <c r="D90" t="s">
-        <v>862</v>
       </c>
     </row>
     <row r="91" spans="2:4">
@@ -8903,10 +8900,10 @@
         <v>270</v>
       </c>
       <c r="C91" s="2" t="s">
+        <v>862</v>
+      </c>
+      <c r="D91" t="s">
         <v>863</v>
-      </c>
-      <c r="D91" t="s">
-        <v>864</v>
       </c>
     </row>
     <row r="92" spans="2:4">
@@ -8914,10 +8911,10 @@
         <v>273</v>
       </c>
       <c r="C92" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="D92" t="s">
         <v>865</v>
-      </c>
-      <c r="D92" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="93" spans="2:4">
@@ -8925,10 +8922,10 @@
         <v>276</v>
       </c>
       <c r="C93" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="D93" t="s">
         <v>867</v>
-      </c>
-      <c r="D93" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="94" spans="2:4">
@@ -8936,10 +8933,10 @@
         <v>279</v>
       </c>
       <c r="C94" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="D94" t="s">
         <v>869</v>
-      </c>
-      <c r="D94" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="95" spans="2:4">
@@ -8947,10 +8944,10 @@
         <v>282</v>
       </c>
       <c r="C95" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="D95" t="s">
         <v>871</v>
-      </c>
-      <c r="D95" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="96" spans="2:4">
@@ -8958,7 +8955,7 @@
         <v>285</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="D96" t="s">
         <v>680</v>
@@ -8969,10 +8966,10 @@
         <v>288</v>
       </c>
       <c r="C97" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="D97" t="s">
         <v>874</v>
-      </c>
-      <c r="D97" t="s">
-        <v>875</v>
       </c>
     </row>
     <row r="98" spans="2:4">
@@ -8980,10 +8977,10 @@
         <v>291</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D98" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="99" spans="2:4">
@@ -8991,10 +8988,10 @@
         <v>294</v>
       </c>
       <c r="C99" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="D99" t="s">
         <v>877</v>
-      </c>
-      <c r="D99" t="s">
-        <v>878</v>
       </c>
     </row>
     <row r="100" spans="2:4">
@@ -9002,10 +8999,10 @@
         <v>297</v>
       </c>
       <c r="C100" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="D100" t="s">
         <v>879</v>
-      </c>
-      <c r="D100" t="s">
-        <v>880</v>
       </c>
     </row>
     <row r="101" spans="2:4">
@@ -9013,10 +9010,10 @@
         <v>300</v>
       </c>
       <c r="C101" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="D101" t="s">
         <v>881</v>
-      </c>
-      <c r="D101" t="s">
-        <v>882</v>
       </c>
     </row>
   </sheetData>
@@ -9055,7 +9052,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D2" t="s">
         <v>498</v>
@@ -9066,10 +9063,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="D3" t="s">
         <v>884</v>
-      </c>
-      <c r="D3" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -9077,10 +9074,10 @@
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="D4" t="s">
         <v>886</v>
-      </c>
-      <c r="D4" t="s">
-        <v>887</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -9088,10 +9085,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="D5" t="s">
         <v>888</v>
-      </c>
-      <c r="D5" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -9099,10 +9096,10 @@
         <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="D6" t="s">
         <v>890</v>
-      </c>
-      <c r="D6" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="7" spans="2:4">
@@ -9110,10 +9107,10 @@
         <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="D7" t="s">
         <v>892</v>
-      </c>
-      <c r="D7" t="s">
-        <v>893</v>
       </c>
     </row>
     <row r="8" spans="2:4">
@@ -9121,10 +9118,10 @@
         <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="D8" t="s">
         <v>894</v>
-      </c>
-      <c r="D8" t="s">
-        <v>895</v>
       </c>
     </row>
     <row r="9" spans="2:4">
@@ -9132,10 +9129,10 @@
         <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="D9" t="s">
         <v>896</v>
-      </c>
-      <c r="D9" t="s">
-        <v>897</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -9143,10 +9140,10 @@
         <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="D10" t="s">
         <v>898</v>
-      </c>
-      <c r="D10" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="11" spans="2:4">
@@ -9154,10 +9151,10 @@
         <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="D11" t="s">
         <v>900</v>
-      </c>
-      <c r="D11" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="12" spans="2:4">
@@ -9165,10 +9162,10 @@
         <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="D12" t="s">
         <v>902</v>
-      </c>
-      <c r="D12" t="s">
-        <v>903</v>
       </c>
     </row>
     <row r="13" spans="2:4">
@@ -9176,10 +9173,10 @@
         <v>36</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="D13" t="s">
         <v>904</v>
-      </c>
-      <c r="D13" t="s">
-        <v>905</v>
       </c>
     </row>
     <row r="14" spans="2:4">
@@ -9187,10 +9184,10 @@
         <v>39</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="D14" t="s">
         <v>906</v>
-      </c>
-      <c r="D14" t="s">
-        <v>907</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -9198,10 +9195,10 @@
         <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="D15" t="s">
         <v>908</v>
-      </c>
-      <c r="D15" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="16" spans="2:4">
@@ -9209,10 +9206,10 @@
         <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="D16" t="s">
         <v>910</v>
-      </c>
-      <c r="D16" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -9220,10 +9217,10 @@
         <v>48</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="D17" t="s">
         <v>912</v>
-      </c>
-      <c r="D17" t="s">
-        <v>913</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -9231,10 +9228,10 @@
         <v>51</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="D18" t="s">
         <v>914</v>
-      </c>
-      <c r="D18" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -9242,10 +9239,10 @@
         <v>54</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="D19" t="s">
         <v>916</v>
-      </c>
-      <c r="D19" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -9253,10 +9250,10 @@
         <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="D20" t="s">
         <v>918</v>
-      </c>
-      <c r="D20" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -9264,10 +9261,10 @@
         <v>60</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="D21" t="s">
         <v>920</v>
-      </c>
-      <c r="D21" t="s">
-        <v>921</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -9275,10 +9272,10 @@
         <v>63</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="D22" t="s">
         <v>922</v>
-      </c>
-      <c r="D22" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -9286,10 +9283,10 @@
         <v>66</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="D23" t="s">
         <v>924</v>
-      </c>
-      <c r="D23" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="24" spans="2:4">
@@ -9297,10 +9294,10 @@
         <v>69</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="D24" t="s">
         <v>926</v>
-      </c>
-      <c r="D24" t="s">
-        <v>927</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -9308,10 +9305,10 @@
         <v>72</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="D25" t="s">
         <v>928</v>
-      </c>
-      <c r="D25" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -9319,10 +9316,10 @@
         <v>75</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="D26" t="s">
         <v>930</v>
-      </c>
-      <c r="D26" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -9330,10 +9327,10 @@
         <v>78</v>
       </c>
       <c r="C27" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="D27" t="s">
         <v>932</v>
-      </c>
-      <c r="D27" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -9341,10 +9338,10 @@
         <v>81</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="D28" t="s">
         <v>934</v>
-      </c>
-      <c r="D28" t="s">
-        <v>935</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -9352,10 +9349,10 @@
         <v>84</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="D29" t="s">
         <v>936</v>
-      </c>
-      <c r="D29" t="s">
-        <v>937</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -9363,10 +9360,10 @@
         <v>87</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="D30" t="s">
         <v>938</v>
-      </c>
-      <c r="D30" t="s">
-        <v>939</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -9374,10 +9371,10 @@
         <v>90</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="D31" t="s">
         <v>940</v>
-      </c>
-      <c r="D31" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -9385,10 +9382,10 @@
         <v>93</v>
       </c>
       <c r="C32" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="D32" t="s">
         <v>942</v>
-      </c>
-      <c r="D32" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -9396,10 +9393,10 @@
         <v>96</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="D33" t="s">
         <v>944</v>
-      </c>
-      <c r="D33" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -9407,10 +9404,10 @@
         <v>99</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="D34" t="s">
         <v>946</v>
-      </c>
-      <c r="D34" t="s">
-        <v>947</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -9418,10 +9415,10 @@
         <v>102</v>
       </c>
       <c r="C35" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="D35" t="s">
         <v>948</v>
-      </c>
-      <c r="D35" t="s">
-        <v>949</v>
       </c>
     </row>
     <row r="36" spans="2:4">
@@ -9429,10 +9426,10 @@
         <v>105</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="D36" t="s">
         <v>950</v>
-      </c>
-      <c r="D36" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="37" spans="2:4">
@@ -9440,10 +9437,10 @@
         <v>108</v>
       </c>
       <c r="C37" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="D37" t="s">
         <v>952</v>
-      </c>
-      <c r="D37" t="s">
-        <v>953</v>
       </c>
     </row>
     <row r="38" spans="2:4">
@@ -9451,10 +9448,10 @@
         <v>111</v>
       </c>
       <c r="C38" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="D38" t="s">
         <v>954</v>
-      </c>
-      <c r="D38" t="s">
-        <v>955</v>
       </c>
     </row>
     <row r="39" spans="2:4">
@@ -9462,10 +9459,10 @@
         <v>114</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="D39" t="s">
         <v>956</v>
-      </c>
-      <c r="D39" t="s">
-        <v>957</v>
       </c>
     </row>
     <row r="40" spans="2:4">
@@ -9473,10 +9470,10 @@
         <v>117</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="D40" t="s">
         <v>958</v>
-      </c>
-      <c r="D40" t="s">
-        <v>959</v>
       </c>
     </row>
     <row r="41" spans="2:4">
@@ -9484,10 +9481,10 @@
         <v>120</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="D41" t="s">
         <v>960</v>
-      </c>
-      <c r="D41" t="s">
-        <v>961</v>
       </c>
     </row>
     <row r="42" spans="2:4">
@@ -9495,10 +9492,10 @@
         <v>123</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="D42" t="s">
         <v>962</v>
-      </c>
-      <c r="D42" t="s">
-        <v>963</v>
       </c>
     </row>
     <row r="43" spans="2:4">
@@ -9506,10 +9503,10 @@
         <v>126</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="D43" t="s">
         <v>964</v>
-      </c>
-      <c r="D43" t="s">
-        <v>965</v>
       </c>
     </row>
     <row r="44" spans="2:4">
@@ -9517,10 +9514,10 @@
         <v>129</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="D44" t="s">
         <v>966</v>
-      </c>
-      <c r="D44" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="45" spans="2:4">
@@ -9528,10 +9525,10 @@
         <v>132</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="D45" t="s">
         <v>968</v>
-      </c>
-      <c r="D45" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="46" spans="2:4">
@@ -9539,10 +9536,10 @@
         <v>135</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="D46" t="s">
         <v>970</v>
-      </c>
-      <c r="D46" t="s">
-        <v>971</v>
       </c>
     </row>
     <row r="47" spans="2:4">
@@ -9550,10 +9547,10 @@
         <v>138</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D47" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="48" spans="2:4">
@@ -9561,10 +9558,10 @@
         <v>141</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="D48" t="s">
         <v>973</v>
-      </c>
-      <c r="D48" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="49" spans="2:4">
@@ -9572,10 +9569,10 @@
         <v>144</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D49" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="50" spans="2:4">
@@ -9583,7 +9580,7 @@
         <v>147</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="D50" t="s">
         <v>149</v>
@@ -9594,10 +9591,10 @@
         <v>150</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="D51" t="s">
         <v>977</v>
-      </c>
-      <c r="D51" t="s">
-        <v>978</v>
       </c>
     </row>
     <row r="52" spans="2:4">
@@ -9605,10 +9602,10 @@
         <v>153</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="D52" t="s">
         <v>979</v>
-      </c>
-      <c r="D52" t="s">
-        <v>980</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -9616,10 +9613,10 @@
         <v>156</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="D53" t="s">
         <v>981</v>
-      </c>
-      <c r="D53" t="s">
-        <v>982</v>
       </c>
     </row>
     <row r="54" spans="2:4">
@@ -9627,10 +9624,10 @@
         <v>159</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="D54" t="s">
         <v>983</v>
-      </c>
-      <c r="D54" t="s">
-        <v>984</v>
       </c>
     </row>
     <row r="55" spans="2:4">
@@ -9638,10 +9635,10 @@
         <v>162</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="D55" t="s">
         <v>985</v>
-      </c>
-      <c r="D55" t="s">
-        <v>986</v>
       </c>
     </row>
     <row r="56" spans="2:4">
@@ -9649,10 +9646,10 @@
         <v>165</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="D56" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="57" spans="2:4">
@@ -9660,10 +9657,10 @@
         <v>168</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="D57" t="s">
         <v>988</v>
-      </c>
-      <c r="D57" t="s">
-        <v>989</v>
       </c>
     </row>
     <row r="58" spans="2:4">
@@ -9671,7 +9668,7 @@
         <v>171</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="D58" t="s">
         <v>173</v>
@@ -9682,10 +9679,10 @@
         <v>174</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="D59" t="s">
         <v>991</v>
-      </c>
-      <c r="D59" t="s">
-        <v>992</v>
       </c>
     </row>
     <row r="60" spans="2:4">
@@ -9693,10 +9690,10 @@
         <v>177</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="D60" t="s">
         <v>993</v>
-      </c>
-      <c r="D60" t="s">
-        <v>994</v>
       </c>
     </row>
     <row r="61" spans="2:4">
@@ -9704,10 +9701,10 @@
         <v>180</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="D61" t="s">
         <v>995</v>
-      </c>
-      <c r="D61" t="s">
-        <v>996</v>
       </c>
     </row>
     <row r="62" spans="2:4">
@@ -9715,10 +9712,10 @@
         <v>183</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="D62" t="s">
         <v>997</v>
-      </c>
-      <c r="D62" t="s">
-        <v>998</v>
       </c>
     </row>
     <row r="63" spans="2:4">
@@ -9726,10 +9723,10 @@
         <v>186</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="D63" t="s">
         <v>999</v>
-      </c>
-      <c r="D63" t="s">
-        <v>1000</v>
       </c>
     </row>
     <row r="64" spans="2:4">
@@ -9737,10 +9734,10 @@
         <v>189</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D64" t="s">
         <v>1001</v>
-      </c>
-      <c r="D64" t="s">
-        <v>1002</v>
       </c>
     </row>
     <row r="65" spans="2:4">
@@ -9748,10 +9745,10 @@
         <v>192</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D65" t="s">
         <v>1003</v>
-      </c>
-      <c r="D65" t="s">
-        <v>1004</v>
       </c>
     </row>
     <row r="66" spans="2:4">
@@ -9759,10 +9756,10 @@
         <v>195</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D66" t="s">
         <v>1005</v>
-      </c>
-      <c r="D66" t="s">
-        <v>1006</v>
       </c>
     </row>
     <row r="67" spans="2:4">
@@ -9770,10 +9767,10 @@
         <v>198</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D67" t="s">
         <v>1007</v>
-      </c>
-      <c r="D67" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="68" spans="2:4">
@@ -9781,10 +9778,10 @@
         <v>201</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D68" t="s">
         <v>1009</v>
-      </c>
-      <c r="D68" t="s">
-        <v>1010</v>
       </c>
     </row>
     <row r="69" spans="2:4">
@@ -9792,10 +9789,10 @@
         <v>204</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D69" t="s">
         <v>1011</v>
-      </c>
-      <c r="D69" t="s">
-        <v>1012</v>
       </c>
     </row>
     <row r="70" spans="2:4">
@@ -9803,10 +9800,10 @@
         <v>207</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D70" t="s">
         <v>1013</v>
-      </c>
-      <c r="D70" t="s">
-        <v>1014</v>
       </c>
     </row>
     <row r="71" spans="2:4">
@@ -9814,7 +9811,7 @@
         <v>210</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D71" t="s">
         <v>212</v>
@@ -9825,10 +9822,10 @@
         <v>213</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D72" t="s">
         <v>1016</v>
-      </c>
-      <c r="D72" t="s">
-        <v>1017</v>
       </c>
     </row>
     <row r="73" spans="2:4">
@@ -9836,7 +9833,7 @@
         <v>216</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="D73" t="s">
         <v>218</v>
@@ -9847,10 +9844,10 @@
         <v>219</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="D74" t="s">
         <v>1019</v>
-      </c>
-      <c r="D74" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="75" spans="2:4">
@@ -9858,10 +9855,10 @@
         <v>222</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D75" t="s">
         <v>1021</v>
-      </c>
-      <c r="D75" t="s">
-        <v>1022</v>
       </c>
     </row>
     <row r="76" spans="2:4">
@@ -9869,10 +9866,10 @@
         <v>225</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="D76" t="s">
         <v>1023</v>
-      </c>
-      <c r="D76" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="77" spans="2:4">
@@ -9880,10 +9877,10 @@
         <v>228</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>1024</v>
+      </c>
+      <c r="D77" t="s">
         <v>1025</v>
-      </c>
-      <c r="D77" t="s">
-        <v>1026</v>
       </c>
     </row>
     <row r="78" spans="2:4">
@@ -9891,10 +9888,10 @@
         <v>231</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>1026</v>
+      </c>
+      <c r="D78" t="s">
         <v>1027</v>
-      </c>
-      <c r="D78" t="s">
-        <v>1028</v>
       </c>
     </row>
     <row r="79" spans="2:4">
@@ -9902,10 +9899,10 @@
         <v>234</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="D79" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="80" spans="2:4">
@@ -9913,10 +9910,10 @@
         <v>237</v>
       </c>
       <c r="C80" s="1" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D80" t="s">
         <v>1030</v>
-      </c>
-      <c r="D80" t="s">
-        <v>1031</v>
       </c>
     </row>
     <row r="81" spans="2:4">
@@ -9924,10 +9921,10 @@
         <v>240</v>
       </c>
       <c r="C81" s="1" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D81" t="s">
         <v>1032</v>
-      </c>
-      <c r="D81" t="s">
-        <v>1033</v>
       </c>
     </row>
     <row r="82" spans="2:4">
@@ -9935,10 +9932,10 @@
         <v>243</v>
       </c>
       <c r="C82" s="1" t="s">
+        <v>1033</v>
+      </c>
+      <c r="D82" t="s">
         <v>1034</v>
-      </c>
-      <c r="D82" t="s">
-        <v>1035</v>
       </c>
     </row>
     <row r="83" spans="2:4">
@@ -9946,7 +9943,7 @@
         <v>246</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D83" t="s">
         <v>654</v>
@@ -9957,10 +9954,10 @@
         <v>249</v>
       </c>
       <c r="C84" s="1" t="s">
+        <v>1036</v>
+      </c>
+      <c r="D84" t="s">
         <v>1037</v>
-      </c>
-      <c r="D84" t="s">
-        <v>1038</v>
       </c>
     </row>
     <row r="85" spans="2:4">
@@ -9968,10 +9965,10 @@
         <v>252</v>
       </c>
       <c r="C85" s="1" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D85" t="s">
         <v>1039</v>
-      </c>
-      <c r="D85" t="s">
-        <v>1040</v>
       </c>
     </row>
     <row r="86" spans="2:4">
@@ -9979,10 +9976,10 @@
         <v>255</v>
       </c>
       <c r="C86" s="1" t="s">
+        <v>1040</v>
+      </c>
+      <c r="D86" t="s">
         <v>1041</v>
-      </c>
-      <c r="D86" t="s">
-        <v>1042</v>
       </c>
     </row>
     <row r="87" spans="2:4">
@@ -9990,10 +9987,10 @@
         <v>258</v>
       </c>
       <c r="C87" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="D87" t="s">
         <v>1043</v>
-      </c>
-      <c r="D87" t="s">
-        <v>1044</v>
       </c>
     </row>
     <row r="88" spans="2:4">
@@ -10001,10 +9998,10 @@
         <v>261</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="D88" t="s">
         <v>1045</v>
-      </c>
-      <c r="D88" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="89" spans="2:4">
@@ -10012,10 +10009,10 @@
         <v>264</v>
       </c>
       <c r="C89" s="1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D89" t="s">
         <v>1047</v>
-      </c>
-      <c r="D89" t="s">
-        <v>1048</v>
       </c>
     </row>
     <row r="90" spans="2:4">
@@ -10023,10 +10020,10 @@
         <v>267</v>
       </c>
       <c r="C90" s="1" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D90" t="s">
         <v>1049</v>
-      </c>
-      <c r="D90" t="s">
-        <v>1050</v>
       </c>
     </row>
     <row r="91" spans="2:4">
@@ -10034,10 +10031,10 @@
         <v>270</v>
       </c>
       <c r="C91" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D91" t="s">
         <v>1051</v>
-      </c>
-      <c r="D91" t="s">
-        <v>1052</v>
       </c>
     </row>
     <row r="92" spans="2:4">
@@ -10045,10 +10042,10 @@
         <v>273</v>
       </c>
       <c r="C92" s="1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D92" t="s">
         <v>1053</v>
-      </c>
-      <c r="D92" t="s">
-        <v>1054</v>
       </c>
     </row>
     <row r="93" spans="2:4">
@@ -10056,10 +10053,10 @@
         <v>276</v>
       </c>
       <c r="C93" s="1" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D93" t="s">
         <v>1055</v>
-      </c>
-      <c r="D93" t="s">
-        <v>1056</v>
       </c>
     </row>
     <row r="94" spans="2:4">
@@ -10067,10 +10064,10 @@
         <v>279</v>
       </c>
       <c r="C94" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D94" t="s">
         <v>1057</v>
-      </c>
-      <c r="D94" t="s">
-        <v>1058</v>
       </c>
     </row>
     <row r="95" spans="2:4">
@@ -10078,10 +10075,10 @@
         <v>282</v>
       </c>
       <c r="C95" s="1" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D95" t="s">
         <v>1059</v>
-      </c>
-      <c r="D95" t="s">
-        <v>1060</v>
       </c>
     </row>
     <row r="96" spans="2:4">
@@ -10089,10 +10086,10 @@
         <v>285</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>1060</v>
+      </c>
+      <c r="D96" t="s">
         <v>1061</v>
-      </c>
-      <c r="D96" t="s">
-        <v>1062</v>
       </c>
     </row>
     <row r="97" spans="2:4">
@@ -10100,10 +10097,10 @@
         <v>288</v>
       </c>
       <c r="C97" s="1" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D97" t="s">
         <v>1063</v>
-      </c>
-      <c r="D97" t="s">
-        <v>1064</v>
       </c>
     </row>
     <row r="98" spans="2:4">
@@ -10111,10 +10108,10 @@
         <v>291</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D98" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="99" spans="2:4">
@@ -10122,10 +10119,10 @@
         <v>294</v>
       </c>
       <c r="C99" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D99" t="s">
         <v>1066</v>
-      </c>
-      <c r="D99" t="s">
-        <v>1067</v>
       </c>
     </row>
     <row r="100" spans="2:4">
@@ -10133,10 +10130,10 @@
         <v>297</v>
       </c>
       <c r="C100" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D100" t="s">
         <v>1068</v>
-      </c>
-      <c r="D100" t="s">
-        <v>1069</v>
       </c>
     </row>
     <row r="101" spans="2:4">
@@ -10144,10 +10141,10 @@
         <v>300</v>
       </c>
       <c r="C101" s="1" t="s">
+        <v>1069</v>
+      </c>
+      <c r="D101" t="s">
         <v>1070</v>
-      </c>
-      <c r="D101" t="s">
-        <v>1071</v>
       </c>
     </row>
   </sheetData>

</xml_diff>